<commit_message>
added animation and start page
</commit_message>
<xml_diff>
--- a/Sprites.xlsx
+++ b/Sprites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\NTU Modules\ECE2035 Programming for Hardware-Software Systems\P2\ECE2035-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65F6B9A-119A-48D2-A595-2582C024A3E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AF4837-FB45-4230-A674-7474E7998672}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E4DF6BA-80E3-4355-8406-1DC646130C45}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="15">
   <si>
     <t>PLAYER 1</t>
   </si>
@@ -188,15 +188,46 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -506,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EDA916-A6BE-428E-83F9-9FD5319B504D}">
-  <dimension ref="A2:BU40"/>
+  <dimension ref="A2:BU38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="BV10" sqref="BV10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="64" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,84 +555,84 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:73" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="N2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="N2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Z2" s="9" t="s">
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Z2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AL2" s="9" t="s">
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AL2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9"/>
-      <c r="AP2" s="9"/>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AX2" s="9" t="s">
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AX2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BJ2" s="9" t="s">
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BJ2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="BK2" s="9"/>
-      <c r="BL2" s="9"/>
-      <c r="BM2" s="9"/>
-      <c r="BN2" s="9"/>
-      <c r="BO2" s="9"/>
-      <c r="BP2" s="9"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="9"/>
-      <c r="BS2" s="9"/>
-      <c r="BT2" s="9"/>
+      <c r="BK2" s="10"/>
+      <c r="BL2" s="10"/>
+      <c r="BM2" s="10"/>
+      <c r="BN2" s="10"/>
+      <c r="BO2" s="10"/>
+      <c r="BP2" s="10"/>
+      <c r="BQ2" s="10"/>
+      <c r="BR2" s="10"/>
+      <c r="BS2" s="10"/>
+      <c r="BT2" s="10"/>
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1238,19 +1269,19 @@
       <c r="BL6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BM6" s="10" t="s">
+      <c r="BM6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BN6" s="10" t="s">
+      <c r="BN6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BO6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="BP6" s="10" t="s">
+      <c r="BP6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BQ6" s="10" t="s">
+      <c r="BQ6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BR6" s="1" t="s">
@@ -1462,13 +1493,13 @@
       <c r="BM7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BN7" s="10" t="s">
+      <c r="BN7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BO7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="BP7" s="10" t="s">
+      <c r="BP7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BQ7" s="1" t="s">
@@ -1683,13 +1714,13 @@
       <c r="BM8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BN8" s="10" t="s">
+      <c r="BN8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BO8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="BP8" s="10" t="s">
+      <c r="BP8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BQ8" s="1" t="s">
@@ -1901,7 +1932,7 @@
       <c r="BL9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BM9" s="10" t="s">
+      <c r="BM9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BN9" s="5" t="s">
@@ -1913,7 +1944,7 @@
       <c r="BP9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="BQ9" s="10" t="s">
+      <c r="BQ9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BR9" s="1" t="s">
@@ -2119,7 +2150,7 @@
       <c r="BK10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BL10" s="10" t="s">
+      <c r="BL10" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BM10" s="5" t="s">
@@ -2137,7 +2168,7 @@
       <c r="BQ10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="BR10" s="10" t="s">
+      <c r="BR10" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BS10" s="1" t="s">
@@ -2340,7 +2371,7 @@
       <c r="BK11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BL11" s="10" t="s">
+      <c r="BL11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BM11" s="5" t="s">
@@ -2358,7 +2389,7 @@
       <c r="BQ11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="BR11" s="10" t="s">
+      <c r="BR11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BS11" s="1" t="s">
@@ -2558,7 +2589,7 @@
       <c r="BJ12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BK12" s="10" t="s">
+      <c r="BK12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BL12" s="5" t="s">
@@ -2582,7 +2613,7 @@
       <c r="BR12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="BS12" s="10" t="s">
+      <c r="BS12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BT12" s="1" t="s">
@@ -2779,7 +2810,7 @@
       <c r="BJ13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BK13" s="10" t="s">
+      <c r="BK13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BL13" s="5" t="s">
@@ -2803,7 +2834,7 @@
       <c r="BR13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="BS13" s="10" t="s">
+      <c r="BS13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BT13" s="1" t="s">
@@ -3000,31 +3031,31 @@
       <c r="BJ14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BK14" s="10" t="s">
+      <c r="BK14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BL14" s="10" t="s">
+      <c r="BL14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BM14" s="10" t="s">
+      <c r="BM14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BN14" s="10" t="s">
+      <c r="BN14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BO14" s="10" t="s">
+      <c r="BO14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BP14" s="10" t="s">
+      <c r="BP14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BQ14" s="10" t="s">
+      <c r="BQ14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BR14" s="10" t="s">
+      <c r="BR14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="BS14" s="10" t="s">
+      <c r="BS14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="BT14" s="1" t="s">
@@ -3034,9 +3065,2919 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L40" t="s">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AP16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AV16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BM16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BO16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BQ16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AP17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BM17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BQ17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BM18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BQ18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BR18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP19" s="8">
+        <v>5</v>
+      </c>
+      <c r="AQ19" s="8">
+        <v>5</v>
+      </c>
+      <c r="AR19" s="8">
+        <v>5</v>
+      </c>
+      <c r="AS19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI19" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BM19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BQ19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO20" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP20" s="8">
+        <v>5</v>
+      </c>
+      <c r="AQ20" s="8">
+        <v>5</v>
+      </c>
+      <c r="AR20" s="8">
+        <v>5</v>
+      </c>
+      <c r="AS20" s="8">
+        <v>5</v>
+      </c>
+      <c r="AT20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI20" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BM20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BQ20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>5</v>
+      </c>
+      <c r="R21" s="8">
+        <v>5</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO21" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ21" s="8">
+        <v>5</v>
+      </c>
+      <c r="AR21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS21" s="8">
+        <v>5</v>
+      </c>
+      <c r="AT21" s="8">
+        <v>5</v>
+      </c>
+      <c r="AU21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI21" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BM21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BR21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BS21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>5</v>
+      </c>
+      <c r="R22" s="8">
+        <v>5</v>
+      </c>
+      <c r="S22" s="8">
+        <v>5</v>
+      </c>
+      <c r="T22" s="8">
+        <v>5</v>
+      </c>
+      <c r="U22" s="8">
+        <v>5</v>
+      </c>
+      <c r="V22" s="8">
+        <v>5</v>
+      </c>
+      <c r="W22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN22" s="8">
+        <v>5</v>
+      </c>
+      <c r="AO22" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ22" s="8">
+        <v>5</v>
+      </c>
+      <c r="AR22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS22" s="8">
+        <v>5</v>
+      </c>
+      <c r="AT22" s="8">
+        <v>5</v>
+      </c>
+      <c r="AU22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AV22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI22" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BM22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BS22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>5</v>
+      </c>
+      <c r="R23" s="8">
+        <v>5</v>
+      </c>
+      <c r="S23" s="8">
+        <v>5</v>
+      </c>
+      <c r="T23" s="8">
+        <v>5</v>
+      </c>
+      <c r="U23" s="8">
+        <v>5</v>
+      </c>
+      <c r="V23" s="8">
+        <v>5</v>
+      </c>
+      <c r="W23" s="8">
+        <v>5</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AO23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AQ23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AR23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AS23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AT23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AU23" s="8">
+        <v>5</v>
+      </c>
+      <c r="AV23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI23" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BM23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BS23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BT23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN24" s="8">
+        <v>5</v>
+      </c>
+      <c r="AO24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP24" s="8">
+        <v>5</v>
+      </c>
+      <c r="AQ24" s="8">
+        <v>5</v>
+      </c>
+      <c r="AR24" s="8">
+        <v>5</v>
+      </c>
+      <c r="AS24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT24" s="8">
+        <v>5</v>
+      </c>
+      <c r="AU24" s="8">
+        <v>5</v>
+      </c>
+      <c r="AV24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW24" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI24" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BT24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM25" s="8">
+        <v>5</v>
+      </c>
+      <c r="AN25" s="8">
+        <v>5</v>
+      </c>
+      <c r="AO25" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS25" s="8">
+        <v>5</v>
+      </c>
+      <c r="AT25" s="8">
+        <v>5</v>
+      </c>
+      <c r="AU25" s="8">
+        <v>5</v>
+      </c>
+      <c r="AV25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW25" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI25" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BT25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" t="s">
+        <v>12</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AN26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AO26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AQ26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AR26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AS26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AT26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AU26" s="8">
+        <v>5</v>
+      </c>
+      <c r="AV26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW26" t="s">
+        <v>12</v>
+      </c>
+      <c r="BI26" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BM26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BN26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BP26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BQ26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BR26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BS26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="BT26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BU26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:73" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S35" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T35" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" t="s">
+        <v>12</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" t="s">
+        <v>12</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3048,6 +5989,10 @@
     <mergeCell ref="AL2:AV2"/>
     <mergeCell ref="AX2:BH2"/>
   </mergeCells>
+  <conditionalFormatting sqref="I36:I37">
+    <cfRule type="uniqueValues" dxfId="1" priority="1"/>
+    <cfRule type="uniqueValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add footprint and fix range graphics
</commit_message>
<xml_diff>
--- a/Sprites.xlsx
+++ b/Sprites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\NTU Modules\ECE2035 Programming for Hardware-Software Systems\P2\ECE2035-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AF4837-FB45-4230-A674-7474E7998672}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6E2139-D670-4738-8E3D-04492A844B25}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E4DF6BA-80E3-4355-8406-1DC646130C45}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="16">
   <si>
     <t>PLAYER 1</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>FOOT</t>
   </si>
 </sst>
 </file>
@@ -196,17 +199,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -537,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EDA916-A6BE-428E-83F9-9FD5319B504D}">
-  <dimension ref="A2:BU38"/>
+  <dimension ref="A2:CG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="64" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T43" sqref="T43"/>
+    <sheetView tabSelected="1" topLeftCell="O3" zoomScale="80" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BX29" sqref="BX29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,9 +545,10 @@
     <col min="38" max="48" width="2.6640625" customWidth="1"/>
     <col min="50" max="60" width="2.6640625" customWidth="1"/>
     <col min="62" max="72" width="2.6640625" customWidth="1"/>
+    <col min="74" max="84" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
@@ -633,8 +627,21 @@
       <c r="BR2" s="10"/>
       <c r="BS2" s="10"/>
       <c r="BT2" s="10"/>
+      <c r="BV2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BW2" s="10"/>
+      <c r="BX2" s="10"/>
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="10"/>
+      <c r="CB2" s="10"/>
+      <c r="CC2" s="10"/>
+      <c r="CD2" s="10"/>
+      <c r="CE2" s="10"/>
+      <c r="CF2" s="10"/>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -854,8 +861,44 @@
       <c r="BU4" t="s">
         <v>12</v>
       </c>
+      <c r="BV4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CB4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CC4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1075,8 +1118,44 @@
       <c r="BU5" t="s">
         <v>12</v>
       </c>
+      <c r="BV5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CC5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1296,8 +1375,44 @@
       <c r="BU6" t="s">
         <v>12</v>
       </c>
+      <c r="BV6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BX6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CE6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CF6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1517,8 +1632,44 @@
       <c r="BU7" t="s">
         <v>12</v>
       </c>
+      <c r="BV7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BX7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CE7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CF7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1738,8 +1889,44 @@
       <c r="BU8" t="s">
         <v>12</v>
       </c>
+      <c r="BV8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CA8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CB8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CC8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG8" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1959,8 +2146,44 @@
       <c r="BU9" t="s">
         <v>12</v>
       </c>
+      <c r="BV9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CD9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG9" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2180,8 +2403,44 @@
       <c r="BU10" t="s">
         <v>12</v>
       </c>
+      <c r="BV10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BZ10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CD10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2401,8 +2660,44 @@
       <c r="BU11" t="s">
         <v>12</v>
       </c>
+      <c r="BV11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BZ11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CD11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CE11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG11" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2622,8 +2917,44 @@
       <c r="BU12" t="s">
         <v>12</v>
       </c>
+      <c r="BV12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BZ12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CD12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CE12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG12" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2843,8 +3174,44 @@
       <c r="BU13" t="s">
         <v>12</v>
       </c>
+      <c r="BV13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BZ13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CD13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CE13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG13" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3064,8 +3431,44 @@
       <c r="BU14" t="s">
         <v>12</v>
       </c>
+      <c r="BV14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BX14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="BZ14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CA14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CD14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CE14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CG14" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3252,8 +3655,11 @@
       <c r="BU16" t="s">
         <v>12</v>
       </c>
+      <c r="CG16" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3440,8 +3846,11 @@
       <c r="BU17" t="s">
         <v>12</v>
       </c>
+      <c r="CG17" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3628,8 +4037,11 @@
       <c r="BU18" t="s">
         <v>12</v>
       </c>
+      <c r="CG18" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3816,8 +4228,11 @@
       <c r="BU19" t="s">
         <v>12</v>
       </c>
+      <c r="CG19" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4004,8 +4419,11 @@
       <c r="BU20" t="s">
         <v>12</v>
       </c>
+      <c r="CG20" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4192,8 +4610,11 @@
       <c r="BU21" t="s">
         <v>12</v>
       </c>
+      <c r="CG21" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4380,8 +4801,11 @@
       <c r="BU22" t="s">
         <v>12</v>
       </c>
+      <c r="CG22" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -4568,8 +4992,11 @@
       <c r="BU23" t="s">
         <v>12</v>
       </c>
+      <c r="CG23" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4756,8 +5183,11 @@
       <c r="BU24" t="s">
         <v>12</v>
       </c>
+      <c r="CG24" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -4944,8 +5374,11 @@
       <c r="BU25" t="s">
         <v>12</v>
       </c>
+      <c r="CG25" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -5132,8 +5565,11 @@
       <c r="BU26" t="s">
         <v>12</v>
       </c>
+      <c r="CG26" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -5210,7 +5646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -5287,7 +5723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -5364,7 +5800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -5441,7 +5877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -5981,7 +6417,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="BV2:CF2"/>
     <mergeCell ref="BJ2:BT2"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="N2:X2"/>

</xml_diff>